<commit_message>
added component on lcsc list
</commit_message>
<xml_diff>
--- a/Part orders/Fourth order Rastaban-HAT LCSC.xlsx
+++ b/Part orders/Fourth order Rastaban-HAT LCSC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Hardware/Rastaban-HAT/Rastaban-HAT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Part orders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:40009_{59A8B70D-005F-466F-A5A0-CF3E9FC2D459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25956D7E-6B2F-42F3-A0D6-C22411425AB5}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{59A8B70D-005F-466F-A5A0-CF3E9FC2D459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D02AE369-01B3-4B5C-8BCE-EE92D6A7CA1C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rastaban-HAT" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="209">
   <si>
     <t>Collated Components:</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>ORDER THE GREEN PARTS</t>
+  </si>
+  <si>
+    <t>C347423</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1164,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1172,7 +1175,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1530,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1797,7 +1799,7 @@
       <c r="G12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2669,28 +2671,28 @@
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>46</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" s="4"/>
+      <c r="G49" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">

</xml_diff>

<commit_message>
improved routing and connected unconnected tracks
</commit_message>
<xml_diff>
--- a/Part orders/Fourth order Rastaban-HAT LCSC.xlsx
+++ b/Part orders/Fourth order Rastaban-HAT LCSC.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{59A8B70D-005F-466F-A5A0-CF3E9FC2D459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77CB146C-06C7-4255-A91F-3F2BD9F14A34}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rastaban-HAT" sheetId="1" r:id="rId1"/>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>